<commit_message>
Update Chart of Accounts import/export functionality to handle schema changes.  This includes removing reporting fields and updating test data and scripts.
Replit-Commit-Author: Agent
Replit-Commit-Session-Id: f5791d6d-82c7-4faa-bd4a-8030f920af85
Replit-Commit-Screenshot-Url: https://storage.googleapis.com/screenshot-production-us-central1/80550fad-9a85-4035-aa54-a26530837091/10bc7423-e239-4ac9-bb27-aa5b71d897f5.jpg
</commit_message>
<xml_diff>
--- a/test/coa-import-export/valid_import.xlsx
+++ b/test/coa-import-export/valid_import.xlsx
@@ -3,7 +3,7 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <workbookPr codeName="ThisWorkbook"/>
   <sheets>
-    <sheet name="Chart of Accounts" sheetId="1" r:id="rId1"/>
+    <sheet name="CoA Import" sheetId="1" r:id="rId1"/>
   </sheets>
 </workbook>
 </file>
@@ -397,46 +397,46 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:I11"/>
+  <dimension ref="A1:I4"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
   <sheetData>
     <row r="1">
       <c r="A1" t="str">
-        <v>Code</v>
+        <v>code</v>
       </c>
       <c r="B1" t="str">
-        <v>Name</v>
+        <v>name</v>
       </c>
       <c r="C1" t="str">
-        <v>Type</v>
+        <v>type</v>
       </c>
       <c r="D1" t="str">
-        <v>Subtype</v>
+        <v>subtype</v>
       </c>
       <c r="E1" t="str">
-        <v>IsSubledger</v>
+        <v>isSubledger</v>
       </c>
       <c r="F1" t="str">
-        <v>SubledgerType</v>
+        <v>subledgerType</v>
       </c>
       <c r="G1" t="str">
-        <v>Active</v>
+        <v>description</v>
       </c>
       <c r="H1" t="str">
-        <v>Description</v>
+        <v>active</v>
       </c>
       <c r="I1" t="str">
-        <v>ParentCode</v>
+        <v>parentCode</v>
       </c>
     </row>
     <row r="2">
       <c r="A2" t="str">
-        <v>1000</v>
+        <v>9997</v>
       </c>
       <c r="B2" t="str">
-        <v>Test Cash</v>
+        <v>Test Asset Account</v>
       </c>
       <c r="C2" t="str">
         <v>ASSET</v>
@@ -451,27 +451,27 @@
         <v/>
       </c>
       <c r="G2" t="str">
+        <v>Test account for import</v>
+      </c>
+      <c r="H2" t="str">
         <v>true</v>
       </c>
-      <c r="H2" t="str">
-        <v>Cash on hand</v>
-      </c>
       <c r="I2" t="str">
-        <v/>
+        <v>1100</v>
       </c>
     </row>
     <row r="3">
       <c r="A3" t="str">
-        <v>1100</v>
+        <v>9998</v>
       </c>
       <c r="B3" t="str">
-        <v>Test Bank Account</v>
+        <v>Test Liability Account</v>
       </c>
       <c r="C3" t="str">
-        <v>ASSET</v>
+        <v>LIABILITY</v>
       </c>
       <c r="D3" t="str">
-        <v>Current Asset</v>
+        <v>Current Liability</v>
       </c>
       <c r="E3" t="str">
         <v>false</v>
@@ -480,250 +480,47 @@
         <v/>
       </c>
       <c r="G3" t="str">
+        <v>Test account for import</v>
+      </c>
+      <c r="H3" t="str">
         <v>true</v>
       </c>
-      <c r="H3" t="str">
-        <v>Primary bank account</v>
-      </c>
       <c r="I3" t="str">
-        <v>1000</v>
+        <v>2100</v>
       </c>
     </row>
     <row r="4">
       <c r="A4" t="str">
-        <v>1200</v>
+        <v>9999</v>
       </c>
       <c r="B4" t="str">
-        <v>Test Accounts Receivable</v>
+        <v>Test Revenue Account</v>
       </c>
       <c r="C4" t="str">
-        <v>ASSET</v>
+        <v>REVENUE</v>
       </c>
       <c r="D4" t="str">
-        <v>Current Asset</v>
+        <v>Operating Revenue</v>
       </c>
       <c r="E4" t="str">
+        <v>false</v>
+      </c>
+      <c r="F4" t="str">
+        <v/>
+      </c>
+      <c r="G4" t="str">
+        <v>Test account for import</v>
+      </c>
+      <c r="H4" t="str">
         <v>true</v>
       </c>
-      <c r="F4" t="str">
-        <v>Customer</v>
-      </c>
-      <c r="G4" t="str">
-        <v>true</v>
-      </c>
-      <c r="H4" t="str">
-        <v>Amounts owed by customers</v>
-      </c>
       <c r="I4" t="str">
-        <v/>
-      </c>
-    </row>
-    <row r="5">
-      <c r="A5" t="str">
-        <v>2000</v>
-      </c>
-      <c r="B5" t="str">
-        <v>Test Accounts Payable</v>
-      </c>
-      <c r="C5" t="str">
-        <v>LIABILITY</v>
-      </c>
-      <c r="D5" t="str">
-        <v>Current Liability</v>
-      </c>
-      <c r="E5" t="str">
-        <v>true</v>
-      </c>
-      <c r="F5" t="str">
-        <v>Vendor</v>
-      </c>
-      <c r="G5" t="str">
-        <v>true</v>
-      </c>
-      <c r="H5" t="str">
-        <v>Amounts owed to vendors</v>
-      </c>
-      <c r="I5" t="str">
-        <v/>
-      </c>
-    </row>
-    <row r="6">
-      <c r="A6" t="str">
-        <v>2100</v>
-      </c>
-      <c r="B6" t="str">
-        <v>Test Credit Card</v>
-      </c>
-      <c r="C6" t="str">
-        <v>LIABILITY</v>
-      </c>
-      <c r="D6" t="str">
-        <v>Current Liability</v>
-      </c>
-      <c r="E6" t="str">
-        <v>false</v>
-      </c>
-      <c r="F6" t="str">
-        <v/>
-      </c>
-      <c r="G6" t="str">
-        <v>true</v>
-      </c>
-      <c r="H6" t="str">
-        <v>Business credit card</v>
-      </c>
-      <c r="I6" t="str">
-        <v>2000</v>
-      </c>
-    </row>
-    <row r="7">
-      <c r="A7" t="str">
-        <v>3000</v>
-      </c>
-      <c r="B7" t="str">
-        <v>Test Owner Equity</v>
-      </c>
-      <c r="C7" t="str">
-        <v>EQUITY</v>
-      </c>
-      <c r="D7" t="str">
-        <v>Equity</v>
-      </c>
-      <c r="E7" t="str">
-        <v>false</v>
-      </c>
-      <c r="F7" t="str">
-        <v/>
-      </c>
-      <c r="G7" t="str">
-        <v>true</v>
-      </c>
-      <c r="H7" t="str">
-        <v>Owner investment</v>
-      </c>
-      <c r="I7" t="str">
-        <v/>
-      </c>
-    </row>
-    <row r="8">
-      <c r="A8" t="str">
         <v>4000</v>
-      </c>
-      <c r="B8" t="str">
-        <v>Test Sales Revenue</v>
-      </c>
-      <c r="C8" t="str">
-        <v>REVENUE</v>
-      </c>
-      <c r="D8" t="str">
-        <v>Operating Revenue</v>
-      </c>
-      <c r="E8" t="str">
-        <v>false</v>
-      </c>
-      <c r="F8" t="str">
-        <v/>
-      </c>
-      <c r="G8" t="str">
-        <v>true</v>
-      </c>
-      <c r="H8" t="str">
-        <v>Revenue from sales</v>
-      </c>
-      <c r="I8" t="str">
-        <v/>
-      </c>
-    </row>
-    <row r="9">
-      <c r="A9" t="str">
-        <v>4100</v>
-      </c>
-      <c r="B9" t="str">
-        <v>Test Service Revenue</v>
-      </c>
-      <c r="C9" t="str">
-        <v>REVENUE</v>
-      </c>
-      <c r="D9" t="str">
-        <v>Operating Revenue</v>
-      </c>
-      <c r="E9" t="str">
-        <v>false</v>
-      </c>
-      <c r="F9" t="str">
-        <v/>
-      </c>
-      <c r="G9" t="str">
-        <v>true</v>
-      </c>
-      <c r="H9" t="str">
-        <v>Revenue from services</v>
-      </c>
-      <c r="I9" t="str">
-        <v>4000</v>
-      </c>
-    </row>
-    <row r="10">
-      <c r="A10" t="str">
-        <v>5000</v>
-      </c>
-      <c r="B10" t="str">
-        <v>Test Rent Expense</v>
-      </c>
-      <c r="C10" t="str">
-        <v>EXPENSE</v>
-      </c>
-      <c r="D10" t="str">
-        <v>Operating Expense</v>
-      </c>
-      <c r="E10" t="str">
-        <v>false</v>
-      </c>
-      <c r="F10" t="str">
-        <v/>
-      </c>
-      <c r="G10" t="str">
-        <v>true</v>
-      </c>
-      <c r="H10" t="str">
-        <v>Office rent</v>
-      </c>
-      <c r="I10" t="str">
-        <v/>
-      </c>
-    </row>
-    <row r="11">
-      <c r="A11" t="str">
-        <v>5100</v>
-      </c>
-      <c r="B11" t="str">
-        <v>Test Utilities Expense</v>
-      </c>
-      <c r="C11" t="str">
-        <v>EXPENSE</v>
-      </c>
-      <c r="D11" t="str">
-        <v>Operating Expense</v>
-      </c>
-      <c r="E11" t="str">
-        <v>false</v>
-      </c>
-      <c r="F11" t="str">
-        <v/>
-      </c>
-      <c r="G11" t="str">
-        <v>true</v>
-      </c>
-      <c r="H11" t="str">
-        <v>Electricity, water, etc.</v>
-      </c>
-      <c r="I11" t="str">
-        <v>5000</v>
       </c>
     </row>
   </sheetData>
   <ignoredErrors>
-    <ignoredError numberStoredAsText="1" sqref="A1:I11"/>
+    <ignoredError numberStoredAsText="1" sqref="A1:I4"/>
   </ignoredErrors>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
Update Chart of Accounts API endpoints and improve import/export functionality.  This includes updated test scripts and data.
Replit-Commit-Author: Agent
Replit-Commit-Session-Id: f5791d6d-82c7-4faa-bd4a-8030f920af85
Replit-Commit-Screenshot-Url: https://storage.googleapis.com/screenshot-production-us-central1/80550fad-9a85-4035-aa54-a26530837091/f6091011-bd69-41ee-ba21-17b6848b2e99.jpg
</commit_message>
<xml_diff>
--- a/test/coa-import-export/valid_import.xlsx
+++ b/test/coa-import-export/valid_import.xlsx
@@ -3,7 +3,7 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <workbookPr codeName="ThisWorkbook"/>
   <sheets>
-    <sheet name="CoA Import" sheetId="1" r:id="rId1"/>
+    <sheet name="Chart of Accounts" sheetId="1" r:id="rId1"/>
   </sheets>
 </workbook>
 </file>
@@ -397,46 +397,46 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:I4"/>
+  <dimension ref="A1:I11"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
   <sheetData>
     <row r="1">
       <c r="A1" t="str">
-        <v>code</v>
+        <v>Code</v>
       </c>
       <c r="B1" t="str">
-        <v>name</v>
+        <v>Name</v>
       </c>
       <c r="C1" t="str">
-        <v>type</v>
+        <v>Type</v>
       </c>
       <c r="D1" t="str">
-        <v>subtype</v>
+        <v>Subtype</v>
       </c>
       <c r="E1" t="str">
-        <v>isSubledger</v>
+        <v>IsSubledger</v>
       </c>
       <c r="F1" t="str">
-        <v>subledgerType</v>
+        <v>SubledgerType</v>
       </c>
       <c r="G1" t="str">
-        <v>description</v>
+        <v>Active</v>
       </c>
       <c r="H1" t="str">
-        <v>active</v>
+        <v>Description</v>
       </c>
       <c r="I1" t="str">
-        <v>parentCode</v>
+        <v>ParentCode</v>
       </c>
     </row>
     <row r="2">
       <c r="A2" t="str">
-        <v>9997</v>
+        <v>1000</v>
       </c>
       <c r="B2" t="str">
-        <v>Test Asset Account</v>
+        <v>Test Cash</v>
       </c>
       <c r="C2" t="str">
         <v>ASSET</v>
@@ -451,27 +451,27 @@
         <v/>
       </c>
       <c r="G2" t="str">
-        <v>Test account for import</v>
+        <v>true</v>
       </c>
       <c r="H2" t="str">
-        <v>true</v>
+        <v>Cash on hand</v>
       </c>
       <c r="I2" t="str">
-        <v>1100</v>
+        <v/>
       </c>
     </row>
     <row r="3">
       <c r="A3" t="str">
-        <v>9998</v>
+        <v>1100</v>
       </c>
       <c r="B3" t="str">
-        <v>Test Liability Account</v>
+        <v>Test Bank Account</v>
       </c>
       <c r="C3" t="str">
-        <v>LIABILITY</v>
+        <v>ASSET</v>
       </c>
       <c r="D3" t="str">
-        <v>Current Liability</v>
+        <v>Current Asset</v>
       </c>
       <c r="E3" t="str">
         <v>false</v>
@@ -480,47 +480,250 @@
         <v/>
       </c>
       <c r="G3" t="str">
-        <v>Test account for import</v>
+        <v>true</v>
       </c>
       <c r="H3" t="str">
-        <v>true</v>
+        <v>Primary bank account</v>
       </c>
       <c r="I3" t="str">
-        <v>2100</v>
+        <v>1000</v>
       </c>
     </row>
     <row r="4">
       <c r="A4" t="str">
-        <v>9999</v>
+        <v>1200</v>
       </c>
       <c r="B4" t="str">
-        <v>Test Revenue Account</v>
+        <v>Test Accounts Receivable</v>
       </c>
       <c r="C4" t="str">
+        <v>ASSET</v>
+      </c>
+      <c r="D4" t="str">
+        <v>Current Asset</v>
+      </c>
+      <c r="E4" t="str">
+        <v>true</v>
+      </c>
+      <c r="F4" t="str">
+        <v>Customer</v>
+      </c>
+      <c r="G4" t="str">
+        <v>true</v>
+      </c>
+      <c r="H4" t="str">
+        <v>Amounts owed by customers</v>
+      </c>
+      <c r="I4" t="str">
+        <v/>
+      </c>
+    </row>
+    <row r="5">
+      <c r="A5" t="str">
+        <v>2000</v>
+      </c>
+      <c r="B5" t="str">
+        <v>Test Accounts Payable</v>
+      </c>
+      <c r="C5" t="str">
+        <v>LIABILITY</v>
+      </c>
+      <c r="D5" t="str">
+        <v>Current Liability</v>
+      </c>
+      <c r="E5" t="str">
+        <v>true</v>
+      </c>
+      <c r="F5" t="str">
+        <v>Vendor</v>
+      </c>
+      <c r="G5" t="str">
+        <v>true</v>
+      </c>
+      <c r="H5" t="str">
+        <v>Amounts owed to vendors</v>
+      </c>
+      <c r="I5" t="str">
+        <v/>
+      </c>
+    </row>
+    <row r="6">
+      <c r="A6" t="str">
+        <v>2100</v>
+      </c>
+      <c r="B6" t="str">
+        <v>Test Credit Card</v>
+      </c>
+      <c r="C6" t="str">
+        <v>LIABILITY</v>
+      </c>
+      <c r="D6" t="str">
+        <v>Current Liability</v>
+      </c>
+      <c r="E6" t="str">
+        <v>false</v>
+      </c>
+      <c r="F6" t="str">
+        <v/>
+      </c>
+      <c r="G6" t="str">
+        <v>true</v>
+      </c>
+      <c r="H6" t="str">
+        <v>Business credit card</v>
+      </c>
+      <c r="I6" t="str">
+        <v>2000</v>
+      </c>
+    </row>
+    <row r="7">
+      <c r="A7" t="str">
+        <v>3000</v>
+      </c>
+      <c r="B7" t="str">
+        <v>Test Owner Equity</v>
+      </c>
+      <c r="C7" t="str">
+        <v>EQUITY</v>
+      </c>
+      <c r="D7" t="str">
+        <v>Equity</v>
+      </c>
+      <c r="E7" t="str">
+        <v>false</v>
+      </c>
+      <c r="F7" t="str">
+        <v/>
+      </c>
+      <c r="G7" t="str">
+        <v>true</v>
+      </c>
+      <c r="H7" t="str">
+        <v>Owner investment</v>
+      </c>
+      <c r="I7" t="str">
+        <v/>
+      </c>
+    </row>
+    <row r="8">
+      <c r="A8" t="str">
+        <v>4000</v>
+      </c>
+      <c r="B8" t="str">
+        <v>Test Sales Revenue</v>
+      </c>
+      <c r="C8" t="str">
         <v>REVENUE</v>
       </c>
-      <c r="D4" t="str">
+      <c r="D8" t="str">
         <v>Operating Revenue</v>
       </c>
-      <c r="E4" t="str">
+      <c r="E8" t="str">
         <v>false</v>
       </c>
-      <c r="F4" t="str">
-        <v/>
-      </c>
-      <c r="G4" t="str">
-        <v>Test account for import</v>
-      </c>
-      <c r="H4" t="str">
-        <v>true</v>
-      </c>
-      <c r="I4" t="str">
+      <c r="F8" t="str">
+        <v/>
+      </c>
+      <c r="G8" t="str">
+        <v>true</v>
+      </c>
+      <c r="H8" t="str">
+        <v>Revenue from sales</v>
+      </c>
+      <c r="I8" t="str">
+        <v/>
+      </c>
+    </row>
+    <row r="9">
+      <c r="A9" t="str">
+        <v>4100</v>
+      </c>
+      <c r="B9" t="str">
+        <v>Test Service Revenue</v>
+      </c>
+      <c r="C9" t="str">
+        <v>REVENUE</v>
+      </c>
+      <c r="D9" t="str">
+        <v>Operating Revenue</v>
+      </c>
+      <c r="E9" t="str">
+        <v>false</v>
+      </c>
+      <c r="F9" t="str">
+        <v/>
+      </c>
+      <c r="G9" t="str">
+        <v>true</v>
+      </c>
+      <c r="H9" t="str">
+        <v>Revenue from services</v>
+      </c>
+      <c r="I9" t="str">
         <v>4000</v>
+      </c>
+    </row>
+    <row r="10">
+      <c r="A10" t="str">
+        <v>5000</v>
+      </c>
+      <c r="B10" t="str">
+        <v>Test Rent Expense</v>
+      </c>
+      <c r="C10" t="str">
+        <v>EXPENSE</v>
+      </c>
+      <c r="D10" t="str">
+        <v>Operating Expense</v>
+      </c>
+      <c r="E10" t="str">
+        <v>false</v>
+      </c>
+      <c r="F10" t="str">
+        <v/>
+      </c>
+      <c r="G10" t="str">
+        <v>true</v>
+      </c>
+      <c r="H10" t="str">
+        <v>Office rent</v>
+      </c>
+      <c r="I10" t="str">
+        <v/>
+      </c>
+    </row>
+    <row r="11">
+      <c r="A11" t="str">
+        <v>5100</v>
+      </c>
+      <c r="B11" t="str">
+        <v>Test Utilities Expense</v>
+      </c>
+      <c r="C11" t="str">
+        <v>EXPENSE</v>
+      </c>
+      <c r="D11" t="str">
+        <v>Operating Expense</v>
+      </c>
+      <c r="E11" t="str">
+        <v>false</v>
+      </c>
+      <c r="F11" t="str">
+        <v/>
+      </c>
+      <c r="G11" t="str">
+        <v>true</v>
+      </c>
+      <c r="H11" t="str">
+        <v>Electricity, water, etc.</v>
+      </c>
+      <c r="I11" t="str">
+        <v>5000</v>
       </c>
     </row>
   </sheetData>
   <ignoredErrors>
-    <ignoredError numberStoredAsText="1" sqref="A1:I4"/>
+    <ignoredError numberStoredAsText="1" sqref="A1:I11"/>
   </ignoredErrors>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
Revert changes to Chart of Accounts import UI; previous version was better.
Replit-Commit-Author: Agent
Replit-Commit-Session-Id: 57888831-7d4d-42d4-b189-8571377faa50
Replit-Commit-Screenshot-Url: https://storage.googleapis.com/screenshot-production-us-central1/80550fad-9a85-4035-aa54-a26530837091/fb1a6033-e66a-477b-9d5c-1d564c44ba0e.jpg
</commit_message>
<xml_diff>
--- a/test/coa-import-export/valid_import.xlsx
+++ b/test/coa-import-export/valid_import.xlsx
@@ -3,7 +3,7 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <workbookPr codeName="ThisWorkbook"/>
   <sheets>
-    <sheet name="Chart of Accounts" sheetId="1" r:id="rId1"/>
+    <sheet name="CoA Import" sheetId="1" r:id="rId1"/>
   </sheets>
 </workbook>
 </file>
@@ -397,46 +397,46 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:I11"/>
+  <dimension ref="A1:I4"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
   <sheetData>
     <row r="1">
       <c r="A1" t="str">
-        <v>Code</v>
+        <v>code</v>
       </c>
       <c r="B1" t="str">
-        <v>Name</v>
+        <v>name</v>
       </c>
       <c r="C1" t="str">
-        <v>Type</v>
+        <v>type</v>
       </c>
       <c r="D1" t="str">
-        <v>Subtype</v>
+        <v>subtype</v>
       </c>
       <c r="E1" t="str">
-        <v>IsSubledger</v>
+        <v>isSubledger</v>
       </c>
       <c r="F1" t="str">
-        <v>SubledgerType</v>
+        <v>subledgerType</v>
       </c>
       <c r="G1" t="str">
-        <v>Active</v>
+        <v>description</v>
       </c>
       <c r="H1" t="str">
-        <v>Description</v>
+        <v>active</v>
       </c>
       <c r="I1" t="str">
-        <v>ParentCode</v>
+        <v>parentCode</v>
       </c>
     </row>
     <row r="2">
       <c r="A2" t="str">
-        <v>1000</v>
+        <v>9997</v>
       </c>
       <c r="B2" t="str">
-        <v>Test Cash</v>
+        <v>Test Asset Account</v>
       </c>
       <c r="C2" t="str">
         <v>ASSET</v>
@@ -451,27 +451,27 @@
         <v/>
       </c>
       <c r="G2" t="str">
+        <v>Test account for import</v>
+      </c>
+      <c r="H2" t="str">
         <v>true</v>
       </c>
-      <c r="H2" t="str">
-        <v>Cash on hand</v>
-      </c>
       <c r="I2" t="str">
-        <v/>
+        <v>1100</v>
       </c>
     </row>
     <row r="3">
       <c r="A3" t="str">
-        <v>1100</v>
+        <v>9998</v>
       </c>
       <c r="B3" t="str">
-        <v>Test Bank Account</v>
+        <v>Test Liability Account</v>
       </c>
       <c r="C3" t="str">
-        <v>ASSET</v>
+        <v>LIABILITY</v>
       </c>
       <c r="D3" t="str">
-        <v>Current Asset</v>
+        <v>Current Liability</v>
       </c>
       <c r="E3" t="str">
         <v>false</v>
@@ -480,250 +480,47 @@
         <v/>
       </c>
       <c r="G3" t="str">
+        <v>Test account for import</v>
+      </c>
+      <c r="H3" t="str">
         <v>true</v>
       </c>
-      <c r="H3" t="str">
-        <v>Primary bank account</v>
-      </c>
       <c r="I3" t="str">
-        <v>1000</v>
+        <v>2100</v>
       </c>
     </row>
     <row r="4">
       <c r="A4" t="str">
-        <v>1200</v>
+        <v>9999</v>
       </c>
       <c r="B4" t="str">
-        <v>Test Accounts Receivable</v>
+        <v>Test Revenue Account</v>
       </c>
       <c r="C4" t="str">
-        <v>ASSET</v>
+        <v>REVENUE</v>
       </c>
       <c r="D4" t="str">
-        <v>Current Asset</v>
+        <v>Operating Revenue</v>
       </c>
       <c r="E4" t="str">
+        <v>false</v>
+      </c>
+      <c r="F4" t="str">
+        <v/>
+      </c>
+      <c r="G4" t="str">
+        <v>Test account for import</v>
+      </c>
+      <c r="H4" t="str">
         <v>true</v>
       </c>
-      <c r="F4" t="str">
-        <v>Customer</v>
-      </c>
-      <c r="G4" t="str">
-        <v>true</v>
-      </c>
-      <c r="H4" t="str">
-        <v>Amounts owed by customers</v>
-      </c>
       <c r="I4" t="str">
-        <v/>
-      </c>
-    </row>
-    <row r="5">
-      <c r="A5" t="str">
-        <v>2000</v>
-      </c>
-      <c r="B5" t="str">
-        <v>Test Accounts Payable</v>
-      </c>
-      <c r="C5" t="str">
-        <v>LIABILITY</v>
-      </c>
-      <c r="D5" t="str">
-        <v>Current Liability</v>
-      </c>
-      <c r="E5" t="str">
-        <v>true</v>
-      </c>
-      <c r="F5" t="str">
-        <v>Vendor</v>
-      </c>
-      <c r="G5" t="str">
-        <v>true</v>
-      </c>
-      <c r="H5" t="str">
-        <v>Amounts owed to vendors</v>
-      </c>
-      <c r="I5" t="str">
-        <v/>
-      </c>
-    </row>
-    <row r="6">
-      <c r="A6" t="str">
-        <v>2100</v>
-      </c>
-      <c r="B6" t="str">
-        <v>Test Credit Card</v>
-      </c>
-      <c r="C6" t="str">
-        <v>LIABILITY</v>
-      </c>
-      <c r="D6" t="str">
-        <v>Current Liability</v>
-      </c>
-      <c r="E6" t="str">
-        <v>false</v>
-      </c>
-      <c r="F6" t="str">
-        <v/>
-      </c>
-      <c r="G6" t="str">
-        <v>true</v>
-      </c>
-      <c r="H6" t="str">
-        <v>Business credit card</v>
-      </c>
-      <c r="I6" t="str">
-        <v>2000</v>
-      </c>
-    </row>
-    <row r="7">
-      <c r="A7" t="str">
-        <v>3000</v>
-      </c>
-      <c r="B7" t="str">
-        <v>Test Owner Equity</v>
-      </c>
-      <c r="C7" t="str">
-        <v>EQUITY</v>
-      </c>
-      <c r="D7" t="str">
-        <v>Equity</v>
-      </c>
-      <c r="E7" t="str">
-        <v>false</v>
-      </c>
-      <c r="F7" t="str">
-        <v/>
-      </c>
-      <c r="G7" t="str">
-        <v>true</v>
-      </c>
-      <c r="H7" t="str">
-        <v>Owner investment</v>
-      </c>
-      <c r="I7" t="str">
-        <v/>
-      </c>
-    </row>
-    <row r="8">
-      <c r="A8" t="str">
         <v>4000</v>
-      </c>
-      <c r="B8" t="str">
-        <v>Test Sales Revenue</v>
-      </c>
-      <c r="C8" t="str">
-        <v>REVENUE</v>
-      </c>
-      <c r="D8" t="str">
-        <v>Operating Revenue</v>
-      </c>
-      <c r="E8" t="str">
-        <v>false</v>
-      </c>
-      <c r="F8" t="str">
-        <v/>
-      </c>
-      <c r="G8" t="str">
-        <v>true</v>
-      </c>
-      <c r="H8" t="str">
-        <v>Revenue from sales</v>
-      </c>
-      <c r="I8" t="str">
-        <v/>
-      </c>
-    </row>
-    <row r="9">
-      <c r="A9" t="str">
-        <v>4100</v>
-      </c>
-      <c r="B9" t="str">
-        <v>Test Service Revenue</v>
-      </c>
-      <c r="C9" t="str">
-        <v>REVENUE</v>
-      </c>
-      <c r="D9" t="str">
-        <v>Operating Revenue</v>
-      </c>
-      <c r="E9" t="str">
-        <v>false</v>
-      </c>
-      <c r="F9" t="str">
-        <v/>
-      </c>
-      <c r="G9" t="str">
-        <v>true</v>
-      </c>
-      <c r="H9" t="str">
-        <v>Revenue from services</v>
-      </c>
-      <c r="I9" t="str">
-        <v>4000</v>
-      </c>
-    </row>
-    <row r="10">
-      <c r="A10" t="str">
-        <v>5000</v>
-      </c>
-      <c r="B10" t="str">
-        <v>Test Rent Expense</v>
-      </c>
-      <c r="C10" t="str">
-        <v>EXPENSE</v>
-      </c>
-      <c r="D10" t="str">
-        <v>Operating Expense</v>
-      </c>
-      <c r="E10" t="str">
-        <v>false</v>
-      </c>
-      <c r="F10" t="str">
-        <v/>
-      </c>
-      <c r="G10" t="str">
-        <v>true</v>
-      </c>
-      <c r="H10" t="str">
-        <v>Office rent</v>
-      </c>
-      <c r="I10" t="str">
-        <v/>
-      </c>
-    </row>
-    <row r="11">
-      <c r="A11" t="str">
-        <v>5100</v>
-      </c>
-      <c r="B11" t="str">
-        <v>Test Utilities Expense</v>
-      </c>
-      <c r="C11" t="str">
-        <v>EXPENSE</v>
-      </c>
-      <c r="D11" t="str">
-        <v>Operating Expense</v>
-      </c>
-      <c r="E11" t="str">
-        <v>false</v>
-      </c>
-      <c r="F11" t="str">
-        <v/>
-      </c>
-      <c r="G11" t="str">
-        <v>true</v>
-      </c>
-      <c r="H11" t="str">
-        <v>Electricity, water, etc.</v>
-      </c>
-      <c r="I11" t="str">
-        <v>5000</v>
       </c>
     </row>
   </sheetData>
   <ignoredErrors>
-    <ignoredError numberStoredAsText="1" sqref="A1:I11"/>
+    <ignoredError numberStoredAsText="1" sqref="A1:I4"/>
   </ignoredErrors>
 </worksheet>
 </file>
</xml_diff>